<commit_message>
pom and api code update
</commit_message>
<xml_diff>
--- a/TestData/CustomerDetails.xlsx
+++ b/TestData/CustomerDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Amazon\ParaBankApp\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B795BAF-E20A-49B2-AE8C-32608253A561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7482F1-B583-45F9-8484-20192A314AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51DEB871-E335-499D-BC7A-5EEE083560A5}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Vikesh@123</t>
   </si>
   <si>
-    <t>vikesh115</t>
+    <t>vikesh140</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
API code moification and json validation
</commit_message>
<xml_diff>
--- a/TestData/CustomerDetails.xlsx
+++ b/TestData/CustomerDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Amazon\ParaBankApp\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7482F1-B583-45F9-8484-20192A314AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF872C12-2A29-447A-A6BC-6708D62B61B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51DEB871-E335-499D-BC7A-5EEE083560A5}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Vikesh@123</t>
   </si>
   <si>
-    <t>vikesh140</t>
+    <t>vikesh400</t>
   </si>
 </sst>
 </file>

</xml_diff>